<commit_message>
Added homework 13Feb 2020
</commit_message>
<xml_diff>
--- a/data/0002.xlsx
+++ b/data/0002.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1219"/>
+  <dimension ref="A1:I1220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44099,6 +44099,41 @@
         <v>33900</v>
       </c>
     </row>
+    <row r="1220">
+      <c r="A1220" t="n">
+        <v>1581552000</v>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>2020-02-13</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>0002</t>
+        </is>
+      </c>
+      <c r="D1220" t="inlineStr">
+        <is>
+          <t>KOTRA</t>
+        </is>
+      </c>
+      <c r="E1220" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="F1220" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="G1220" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="H1220" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="I1220" t="n">
+        <v>15200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>